<commit_message>
export intermediate commit 2
</commit_message>
<xml_diff>
--- a/example_1_output.xlsx
+++ b/example_1_output.xlsx
@@ -8,14 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Original Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Processed Data" sheetId="2" r:id="rId2"/>
+    <sheet name="IR data input" sheetId="2" r:id="rId2"/>
+    <sheet name="Credit data input" sheetId="3" r:id="rId3"/>
+    <sheet name="IR Processed Data" sheetId="4" r:id="rId4"/>
+    <sheet name="Credit Processed Data" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="28">
   <si>
     <t>Trade #</t>
   </si>
@@ -600,6 +603,198 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>10000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>10000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>5000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4">
+        <v>0.06</v>
+      </c>
+      <c r="L4">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:12">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -722,4 +917,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:9">
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>